<commit_message>
Working on corpus paper
</commit_message>
<xml_diff>
--- a/responses/test_sample/compare_kappas.xlsx
+++ b/responses/test_sample/compare_kappas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25600" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Set</t>
   </si>
@@ -70,13 +70,31 @@
   </si>
   <si>
     <t>intrans (dev:I01/test:I30)</t>
+  </si>
+  <si>
+    <t>test token agree</t>
+  </si>
+  <si>
+    <t>test token chance agree</t>
+  </si>
+  <si>
+    <t>test token A1 Yes</t>
+  </si>
+  <si>
+    <t>test token A2 Yes</t>
+  </si>
+  <si>
+    <t>test token responses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,6 +114,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,7 +158,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -183,12 +208,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -213,6 +264,18 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -237,6 +300,18 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -566,287 +641,453 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="1">
+        <v>2155</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.81160092800000005</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.785614849187935</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.67799570399999998</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.92389791183294601</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.76366126430724701</v>
+      </c>
+      <c r="I2" s="3">
         <v>0.72595087612464104</v>
       </c>
-      <c r="C2" s="1">
+      <c r="J2" s="3">
         <v>0.94832126854931598</v>
       </c>
-      <c r="D2">
+      <c r="K2" s="1">
         <v>0.78544100062854305</v>
       </c>
-      <c r="E2" s="1">
+      <c r="L2" s="3">
         <v>0.73593225683508501</v>
       </c>
-      <c r="F2" s="1">
+      <c r="M2" s="3">
         <v>0.95125871986660004</v>
       </c>
-      <c r="G2">
-        <v>0.76366126430724701</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="1">
+        <v>2155</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.78004640400000003</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.773549883990719</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.65321332200000004</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.94895591647331701</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.87982784482726195</v>
+      </c>
+      <c r="I3" s="3">
         <v>0.79177415788309802</v>
       </c>
-      <c r="C3" s="1">
+      <c r="J3" s="3">
         <v>0.95684587096289997</v>
       </c>
-      <c r="D3">
+      <c r="K3" s="1">
         <v>0.87398212512413098</v>
       </c>
-      <c r="E3" s="1">
+      <c r="L3" s="3">
         <v>0.80562735424793697</v>
       </c>
-      <c r="F3" s="1">
+      <c r="M3" s="3">
         <v>0.96356525454366204</v>
       </c>
-      <c r="G3">
-        <v>0.87982784482726195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1">
+        <v>2155</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.86310904899999996</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.85522041763340995</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.75796749600000002</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.97819025522041703</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.90988919088438103</v>
+      </c>
+      <c r="I4" s="3">
         <v>0.65856961142341297</v>
       </c>
-      <c r="C4" s="1">
+      <c r="J4" s="3">
         <v>0.89408825978351303</v>
       </c>
-      <c r="D4">
+      <c r="K4" s="1">
         <v>0.87923714976160905</v>
       </c>
-      <c r="E4" s="1">
+      <c r="L4" s="3">
         <v>0.67498940228910498</v>
       </c>
-      <c r="F4" s="1">
+      <c r="M4" s="3">
         <v>0.88747083847948405</v>
       </c>
-      <c r="G4">
-        <v>0.90988919088438103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
+        <v>1293</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.73317865400000004</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.71693735498839894</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.60117032100000001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.92343387499999996</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.80802299998650196</v>
+      </c>
+      <c r="I5" s="3">
         <v>0.89724001554920796</v>
       </c>
-      <c r="C5" s="1">
+      <c r="J5" s="3">
         <v>0.95979854604741499</v>
       </c>
-      <c r="D5">
+      <c r="K5" s="1">
         <v>0.781060954620588</v>
       </c>
-      <c r="E5" s="1">
+      <c r="L5" s="3">
         <v>0.889007450672058</v>
       </c>
-      <c r="F5" s="1">
+      <c r="M5" s="3">
         <v>0.96233911276295803</v>
       </c>
-      <c r="G5">
-        <v>0.80802299998650196</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
+        <v>1293</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.83372003100000003</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.83139984532095901</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.72118953299999999</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.98221190999999997</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.93620006478893103</v>
+      </c>
+      <c r="I6" s="3">
         <v>0.699329504795694</v>
       </c>
-      <c r="C6" s="1">
+      <c r="J6" s="3">
         <v>0.96367708932409102</v>
       </c>
-      <c r="D6">
+      <c r="K6" s="1">
         <v>0.93209001506157496</v>
       </c>
-      <c r="E6" s="1">
+      <c r="L6" s="3">
         <v>0.732474964234621</v>
       </c>
-      <c r="F6" s="1">
+      <c r="M6" s="3">
         <v>0.97010754695228696</v>
       </c>
-      <c r="G6">
-        <v>0.93620006478893103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1">
+        <v>1293</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.86078886300000002</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.87161639597834495</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.76815011399999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.95978344900000001</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.82654056313174296</v>
+      </c>
+      <c r="I7" s="3">
         <v>0.81546947473987696</v>
       </c>
-      <c r="C7" s="1">
+      <c r="J7" s="3">
         <v>0.95431472081218205</v>
       </c>
-      <c r="D7">
+      <c r="K7" s="1">
         <v>0.81183665217830703</v>
       </c>
-      <c r="E7" s="1">
+      <c r="L7" s="3">
         <v>0.82912752501995401</v>
       </c>
-      <c r="F7" s="1">
+      <c r="M7" s="3">
         <v>0.95785787189992699</v>
       </c>
-      <c r="G7">
-        <v>0.82654056313174296</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1">
+        <v>1293</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.81825212700000005</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.786542923433874</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.68238578999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.91879350299999996</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.74432347839842705</v>
+      </c>
+      <c r="I8" s="3">
         <v>0.52277456647398801</v>
       </c>
-      <c r="C8" s="1">
+      <c r="J8" s="3">
         <v>0.943037974683544</v>
       </c>
-      <c r="D8">
-        <v>0.80680411491014603</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="K8" s="1">
+        <v>0.76510933762357303</v>
+      </c>
+      <c r="L8" s="3">
         <v>0.543202615273085</v>
       </c>
-      <c r="F8" s="1">
+      <c r="M8" s="3">
         <v>0.94938650306748396</v>
       </c>
-      <c r="G8">
-        <v>0.79158247413778204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1">
+        <v>1293</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.84532095900000004</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.81747873163186302</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.71926411999999995</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.96751740100000005</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.884294808969038</v>
+      </c>
+      <c r="I9" s="3">
         <v>0.64964937651777599</v>
       </c>
-      <c r="C9" s="1">
+      <c r="J9" s="3">
         <v>0.83937422876623402</v>
       </c>
-      <c r="D9">
+      <c r="K9" s="1">
         <v>0.87499018901312098</v>
       </c>
-      <c r="E9" s="1">
+      <c r="L9" s="3">
         <v>0.65149603675227896</v>
       </c>
-      <c r="F9" s="1">
+      <c r="M9" s="3">
         <v>0.81732216995872498</v>
       </c>
-      <c r="G9">
-        <v>0.884294808969038</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
+        <v>3390</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.82920353999999996</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.81799410029498498</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.70936956699999998</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.94867256600000005</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.82339277726579396</v>
+      </c>
+      <c r="I10" s="3">
         <v>0.78172171702132498</v>
       </c>
-      <c r="C10" s="1">
+      <c r="J10" s="3">
         <v>0.93354080310601995</v>
       </c>
-      <c r="D10">
+      <c r="K10" s="1">
         <v>0.81898662898167296</v>
       </c>
-      <c r="E10" s="1">
+      <c r="L10" s="3">
         <v>0.78932844635356803</v>
       </c>
-      <c r="F10" s="1">
+      <c r="M10" s="3">
         <v>0.93398654188340802</v>
       </c>
-      <c r="G10">
-        <v>0.82339277726579396</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1">
+        <v>3075</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.806178862</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.79024390243902398</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.67773309500000001</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.952195122</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.87190206831294503</v>
+      </c>
+      <c r="I11" s="3">
         <v>0.68538706988945397</v>
       </c>
-      <c r="C11" s="1">
+      <c r="J11" s="3">
         <v>0.93781384828844505</v>
       </c>
-      <c r="D11">
+      <c r="K11" s="1">
         <v>0.86176131430120295</v>
       </c>
-      <c r="E11" s="1">
+      <c r="L11" s="3">
         <v>0.70000411976146504</v>
       </c>
-      <c r="F11" s="1">
+      <c r="M11" s="3">
         <v>0.93842549807646802</v>
       </c>
-      <c r="G11">
-        <v>0.87190206831294503</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>